<commit_message>
recursive IFEQUAL is possible
</commit_message>
<xml_diff>
--- a/test/DIAG/diag.xlsx
+++ b/test/DIAG/diag.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\code\github\CGA_RDL\test\DIAG\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="25596" windowHeight="14976" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>DID_WORK_FOR_DEFINE_0</t>
   </si>
@@ -145,17 +150,114 @@
   </si>
   <si>
     <t>VALUE</t>
+  </si>
+  <si>
+    <t>usingName</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>MI</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>ystem</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>oc</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>udio</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>vif</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>onReceiver</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>[HEADER]Receiver</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>interfaceFunction</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>onSite</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>BnReceiverClass</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>BnvifManagerReceiver</t>
+  </si>
+  <si>
+    <t>BnHMIEventReceiver</t>
+  </si>
+  <si>
+    <t>BnAudioReceiver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -179,7 +281,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -187,9 +289,22 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -224,11 +339,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -247,6 +363,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -283,7 +407,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -627,26 +751,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -654,7 +778,7 @@
       <c r="F1" s="2"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -662,7 +786,7 @@
       <c r="F2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -670,31 +794,31 @@
       <c r="F3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="C4" s="1"/>
       <c r="F4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="C5" s="1"/>
       <c r="F5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="C6" s="1"/>
       <c r="F6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="C7" s="1"/>
       <c r="F7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -704,7 +828,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -714,7 +838,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -725,7 +849,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -736,7 +860,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -748,7 +872,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -759,10 +883,10 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -770,7 +894,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -778,7 +902,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -786,7 +910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -794,19 +918,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -814,7 +938,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
@@ -822,7 +946,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -830,147 +954,203 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B38" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="1" t="s">
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A52" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A54" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A56" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A58" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="1" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A59" s="1" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>